<commit_message>
Add Add Two Numbers
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive\Projects\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EEBB64-7167-4178-BF41-B14B8D71184C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8567A778-47B0-4E7E-A89F-AA3FB5A52062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="495" yWindow="5565" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4095" yWindow="1635" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -39,12 +39,6 @@
     <t>Difficulty</t>
   </si>
   <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Blind75 problem?</t>
   </si>
   <si>
@@ -60,38 +54,9 @@
     <t>Array</t>
   </si>
   <si>
-    <t>https://leetcode.com/problems/two-sum/</t>
-  </si>
-  <si>
     <t>Revisit</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Go through the list and check if </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">target - i </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>exists in the list. Should try use a set</t>
-    </r>
-  </si>
-  <si>
     <t>Longest Common Prefix</t>
   </si>
   <si>
@@ -101,26 +66,35 @@
     <t>No</t>
   </si>
   <si>
-    <t>Go through each string  char by char until you hit a char that doesn't match</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/longest-common-prefix/</t>
-  </si>
-  <si>
     <t>Valid Parentheses</t>
   </si>
   <si>
-    <t>https://leetcode.com/problems/valid-parentheses/</t>
-  </si>
-  <si>
-    <t>Use a stack to keep track of what parethesis we need to check against</t>
+    <t>Local Path</t>
+  </si>
+  <si>
+    <t>1 - Two Sum</t>
+  </si>
+  <si>
+    <t>14 - Longest Common Prefix</t>
+  </si>
+  <si>
+    <t>20 - Valid Parentheses</t>
+  </si>
+  <si>
+    <t>Add Two Numbers</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>2 - Add Two Numbers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,9 +111,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -162,14 +142,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -470,24 +453,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="64.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" customWidth="1"/>
+    <col min="8" max="8" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -495,104 +479,116 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:G4">
+  <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="D2:G5">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -604,20 +600,26 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E4" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F5" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C4" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C5" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B4" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B5" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D5" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{CBB9FB0B-3B21-45D2-8379-0AEC64C38F83}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{42F81A7D-D57B-4524-998E-21D2C489127E}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{DEF253DB-6628-460D-9C1D-83A98000E5A1}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{BEF6569D-A155-4AA1-A66D-2B97BF1658AC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Guess Number Higher or Lower
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive\Projects\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8567A778-47B0-4E7E-A89F-AA3FB5A52062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78896D5-F110-495F-9EF9-F9F5D213AEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4095" yWindow="1635" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11640" yWindow="8265" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>2 - Add Two Numbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Guess Number Higher or Lower</t>
+  </si>
+  <si>
+    <t>374 - Guess Number Higher or Lower</t>
+  </si>
+  <si>
+    <t>Interval</t>
   </si>
 </sst>
 </file>
@@ -453,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,9 +595,32 @@
         <v>20</v>
       </c>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G5">
+  <conditionalFormatting sqref="D2:G6">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -600,16 +632,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F5" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F6" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C5" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C6" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B5" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D5" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -618,8 +650,9 @@
     <hyperlink ref="G3" r:id="rId2" xr:uid="{42F81A7D-D57B-4524-998E-21D2C489127E}"/>
     <hyperlink ref="G4" r:id="rId3" xr:uid="{DEF253DB-6628-460D-9C1D-83A98000E5A1}"/>
     <hyperlink ref="G5" r:id="rId4" xr:uid="{BEF6569D-A155-4AA1-A66D-2B97BF1658AC}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{36913061-5655-4E53-8DDD-4DACC89AB167}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Longest Substring Without Repeating Characters
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive\Projects\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1B46A7-0F02-446E-93CF-B511CF3138A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383B2598-9633-4BC0-A3B6-CAF50BAC7EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14415" yWindow="10140" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10950" yWindow="4875" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>75 - Sort Colors</t>
+  </si>
+  <si>
+    <t>Longest Substring Without Repeating Characters</t>
+  </si>
+  <si>
+    <t>3 - Longest Substring Without Repeating Characters</t>
   </si>
 </sst>
 </file>
@@ -468,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,9 +653,32 @@
         <v>25</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G7">
+  <conditionalFormatting sqref="D2:G8">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -661,16 +690,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F7" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F8" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C7" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C8" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B7" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B8" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D8" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -681,8 +710,9 @@
     <hyperlink ref="G5" r:id="rId4" xr:uid="{BEF6569D-A155-4AA1-A66D-2B97BF1658AC}"/>
     <hyperlink ref="G6" r:id="rId5" xr:uid="{36913061-5655-4E53-8DDD-4DACC89AB167}"/>
     <hyperlink ref="G7" r:id="rId6" xr:uid="{001C4FE1-13C7-45D2-BDCD-8FCFC068E86C}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{3F4389CF-2CA2-4C8A-99C6-D8BA3BEDF1F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId7"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Merge Two Sorted Lists
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive\Projects\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383B2598-9633-4BC0-A3B6-CAF50BAC7EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0731CCA8-9333-4A07-8695-78CC42C4F52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10950" yWindow="4875" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>3 - Longest Substring Without Repeating Characters</t>
+  </si>
+  <si>
+    <t>Merge Two Sorted Lists</t>
+  </si>
+  <si>
+    <t>21 - Merge Two Sorted Lists</t>
+  </si>
+  <si>
+    <t>Medium</t>
   </si>
 </sst>
 </file>
@@ -474,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +561,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -598,7 +607,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
@@ -624,7 +633,7 @@
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>21</v>
@@ -644,7 +653,7 @@
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F7" t="s">
         <v>6</v>
@@ -667,7 +676,7 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F8" t="s">
         <v>6</v>
@@ -676,9 +685,32 @@
         <v>27</v>
       </c>
     </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8">
+  <conditionalFormatting sqref="D2:G8 D9:F9">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -690,16 +722,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F8" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F9" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C8" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C9" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B8" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B9" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D8" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D9" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -711,8 +743,9 @@
     <hyperlink ref="G6" r:id="rId5" xr:uid="{36913061-5655-4E53-8DDD-4DACC89AB167}"/>
     <hyperlink ref="G7" r:id="rId6" xr:uid="{001C4FE1-13C7-45D2-BDCD-8FCFC068E86C}"/>
     <hyperlink ref="G8" r:id="rId7" xr:uid="{3F4389CF-2CA2-4C8A-99C6-D8BA3BEDF1F8}"/>
+    <hyperlink ref="G9" r:id="rId8" xr:uid="{74419FB4-3A35-49B9-908F-71C5BA0BD123}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId8"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Best Time to Buy and Sell Stock and improve Sort Colors solutions
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive\Projects\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AC3D76-2CDE-47EE-87B1-4068E090DEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4E519A-F235-4C35-BDE3-4CD5CF37C90B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12030" yWindow="5235" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>53 - Maximum Subarray</t>
+  </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock</t>
+  </si>
+  <si>
+    <t>121 - Best Time to Buy and Sell Stock</t>
   </si>
 </sst>
 </file>
@@ -522,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,7 +695,7 @@
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
         <v>30</v>
@@ -862,9 +868,32 @@
         <v>43</v>
       </c>
     </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F14">
+  <conditionalFormatting sqref="D2:G8 D9:F15">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -876,16 +905,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F14" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F15" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C14" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C15" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B14" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B15" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D14" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D15" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -903,8 +932,9 @@
     <hyperlink ref="G12" r:id="rId11" xr:uid="{71EEFD7D-C1FD-40C0-A9E4-0B50D1DD5B83}"/>
     <hyperlink ref="G13" r:id="rId12" xr:uid="{B4555292-CF3A-442E-97A2-00E830F8B376}"/>
     <hyperlink ref="G14" r:id="rId13" xr:uid="{F3E487B9-F991-419B-989A-FD6CB2F93741}"/>
+    <hyperlink ref="G15" r:id="rId14" xr:uid="{A41E6C83-EF5C-47D5-9B7E-6C4C37742750}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId14"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Product of Array Except Self
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive\Projects\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5321B482-E58B-496C-8C05-5984BDC787F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C283F1-BF51-4D33-A132-FF980B3C1044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6630" yWindow="4875" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>15 - 3Sum</t>
+  </si>
+  <si>
+    <t>Product of Array Except Self</t>
+  </si>
+  <si>
+    <t>238 - Product of Array Except Self</t>
   </si>
 </sst>
 </file>
@@ -540,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,9 +955,32 @@
         <v>49</v>
       </c>
     </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F17">
+  <conditionalFormatting sqref="D2:G8 D9:F18">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -963,16 +992,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F17" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F18" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C17" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C18" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B17" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B18" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D17" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D18" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -993,8 +1022,9 @@
     <hyperlink ref="G15" r:id="rId14" xr:uid="{A41E6C83-EF5C-47D5-9B7E-6C4C37742750}"/>
     <hyperlink ref="G16" r:id="rId15" xr:uid="{6C567687-2677-4115-9ABA-BF01BEEBD720}"/>
     <hyperlink ref="G17" r:id="rId16" xr:uid="{40C441B0-443A-44DC-B54A-A5E23FF32AB9}"/>
+    <hyperlink ref="G18" r:id="rId17" xr:uid="{A261378B-B013-454B-A71E-7432F6DA377C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId17"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Number of 1 Bits
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive\Projects\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C283F1-BF51-4D33-A132-FF980B3C1044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E54FBD-0DAF-4875-8EFA-1C7B5F7C8582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6630" yWindow="4875" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>238 - Product of Array Except Self</t>
+  </si>
+  <si>
+    <t>Number of 1 Bits</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>191 - Number of 1 Bits</t>
   </si>
 </sst>
 </file>
@@ -546,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,9 +987,32 @@
         <v>51</v>
       </c>
     </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F18">
+  <conditionalFormatting sqref="D2:G8 D9:F19">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -992,16 +1024,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F18" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F19" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C18" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C19" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B18" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B19" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D18" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D19" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1023,8 +1055,9 @@
     <hyperlink ref="G16" r:id="rId15" xr:uid="{6C567687-2677-4115-9ABA-BF01BEEBD720}"/>
     <hyperlink ref="G17" r:id="rId16" xr:uid="{40C441B0-443A-44DC-B54A-A5E23FF32AB9}"/>
     <hyperlink ref="G18" r:id="rId17" xr:uid="{A261378B-B013-454B-A71E-7432F6DA377C}"/>
+    <hyperlink ref="G19" r:id="rId18" xr:uid="{BF0CC3D3-2605-40E1-9CA3-79FC8574FC3D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId18"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Merge Sorted Array
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive\Projects\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63C2375-4D58-45E7-B9A0-2A286CC33891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED81D09-EAA1-4269-B5FF-A6DAF36E5888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6630" yWindow="4875" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>994 - Rotting Oranges</t>
+  </si>
+  <si>
+    <t>Merge Sorted Array</t>
+  </si>
+  <si>
+    <t>88 - Merge Sorted Array</t>
   </si>
 </sst>
 </file>
@@ -573,7 +579,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,10 +1078,27 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
       <c r="C22" t="s">
-        <v>5</v>
-      </c>
-      <c r="G22" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1125,8 +1148,9 @@
     <hyperlink ref="G19" r:id="rId18" xr:uid="{BF0CC3D3-2605-40E1-9CA3-79FC8574FC3D}"/>
     <hyperlink ref="G20" r:id="rId19" xr:uid="{C9FACD27-3404-4D9B-9437-8C15184FC4B6}"/>
     <hyperlink ref="G21" r:id="rId20" xr:uid="{CCE9A262-B607-4A7C-9A6A-6581DD6C4512}"/>
+    <hyperlink ref="G22" r:id="rId21" xr:uid="{E4F8706A-0B92-4C41-B108-4DEE8C8A37CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId21"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Reverse Linked List
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive\Projects\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B713322-0C8F-42AC-B67E-D6BEE2FCA66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543EFB72-91FE-43C0-A22A-ADB5B8515330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15600" yWindow="6090" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6795" yWindow="5565" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -220,6 +220,12 @@
   </si>
   <si>
     <t>70 - Climbing Stairs</t>
+  </si>
+  <si>
+    <t>Reverse Linked List</t>
+  </si>
+  <si>
+    <t>206 - Reverse Linked List</t>
   </si>
 </sst>
 </file>
@@ -585,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,9 +1138,32 @@
         <v>64</v>
       </c>
     </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F23">
+  <conditionalFormatting sqref="D2:G8 D9:F24">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1146,16 +1175,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F23" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F24" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C23" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C24" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B23" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B24" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D23" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D24" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1182,8 +1211,9 @@
     <hyperlink ref="G21" r:id="rId20" xr:uid="{CCE9A262-B607-4A7C-9A6A-6581DD6C4512}"/>
     <hyperlink ref="G22" r:id="rId21" xr:uid="{E4F8706A-0B92-4C41-B108-4DEE8C8A37CD}"/>
     <hyperlink ref="G23" r:id="rId22" xr:uid="{58D31123-FD15-4C4D-8962-39B74B90DB25}"/>
+    <hyperlink ref="G24" r:id="rId23" xr:uid="{DADEBF89-877E-4B81-A5B6-896E937BBB99}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId23"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Sum Root to Leaf Numbers
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive\Projects\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A24D20-E5D2-4305-B85F-C0C385F5C02B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0DC2B4-4026-48F3-BEC0-1A58089D571A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6795" yWindow="5565" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -232,6 +232,12 @@
   </si>
   <si>
     <t>242 - Valid Anagram</t>
+  </si>
+  <si>
+    <t>Sum Root to Leaf Numbers</t>
+  </si>
+  <si>
+    <t>129 - Sum Root to Leaf Numbers</t>
   </si>
 </sst>
 </file>
@@ -597,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,9 +1196,32 @@
         <v>68</v>
       </c>
     </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F25">
+  <conditionalFormatting sqref="D2:G8 D9:F26">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1204,16 +1233,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F25" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F26" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C25" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C26" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B25" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B26" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D25" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D26" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1242,8 +1271,9 @@
     <hyperlink ref="G23" r:id="rId22" xr:uid="{58D31123-FD15-4C4D-8962-39B74B90DB25}"/>
     <hyperlink ref="G24" r:id="rId23" xr:uid="{DADEBF89-877E-4B81-A5B6-896E937BBB99}"/>
     <hyperlink ref="G25" r:id="rId24" xr:uid="{95BEC698-DF81-482B-AC3F-17121E33FBDE}"/>
+    <hyperlink ref="G26" r:id="rId25" xr:uid="{685A88B0-0AA1-41C5-895D-E96213F36150}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId25"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Maximum Depth of Binary Tree
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive\Projects\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0DC2B4-4026-48F3-BEC0-1A58089D571A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58B7D65-39FC-4DE2-BF8B-1DE074B79392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6795" yWindow="5565" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="73">
   <si>
     <t>Name</t>
   </si>
@@ -238,6 +238,12 @@
   </si>
   <si>
     <t>129 - Sum Root to Leaf Numbers</t>
+  </si>
+  <si>
+    <t>Maximum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>104 - Maximum Depth of Binary Tree</t>
   </si>
 </sst>
 </file>
@@ -603,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,9 +1225,32 @@
         <v>70</v>
       </c>
     </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F26">
+  <conditionalFormatting sqref="D2:G8 D9:F27">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1233,16 +1262,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F26" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F27" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C26" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C27" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B26" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B27" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D26" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D27" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1272,8 +1301,9 @@
     <hyperlink ref="G24" r:id="rId23" xr:uid="{DADEBF89-877E-4B81-A5B6-896E937BBB99}"/>
     <hyperlink ref="G25" r:id="rId24" xr:uid="{95BEC698-DF81-482B-AC3F-17121E33FBDE}"/>
     <hyperlink ref="G26" r:id="rId25" xr:uid="{685A88B0-0AA1-41C5-895D-E96213F36150}"/>
+    <hyperlink ref="G27" r:id="rId26" xr:uid="{BDB4480A-330F-41CB-B6B7-8ACA26B8A5F9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId26"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Sum of Left Leaves
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive\Projects\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58B7D65-39FC-4DE2-BF8B-1DE074B79392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F965447-FD45-498A-BCFB-F2F4E5CAD5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6795" yWindow="5565" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11145" yWindow="3885" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="75">
   <si>
     <t>Name</t>
   </si>
@@ -244,6 +244,12 @@
   </si>
   <si>
     <t>104 - Maximum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>Sum of Left Leaves</t>
+  </si>
+  <si>
+    <t>404 - Sum of Left Leaves</t>
   </si>
 </sst>
 </file>
@@ -609,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,9 +1254,32 @@
         <v>72</v>
       </c>
     </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F27">
+  <conditionalFormatting sqref="D2:G8 D9:F28">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1262,16 +1291,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F27" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F28" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C27" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C28" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B27" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B28" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D27" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D28" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1302,8 +1331,9 @@
     <hyperlink ref="G25" r:id="rId24" xr:uid="{95BEC698-DF81-482B-AC3F-17121E33FBDE}"/>
     <hyperlink ref="G26" r:id="rId25" xr:uid="{685A88B0-0AA1-41C5-895D-E96213F36150}"/>
     <hyperlink ref="G27" r:id="rId26" xr:uid="{BDB4480A-330F-41CB-B6B7-8ACA26B8A5F9}"/>
+    <hyperlink ref="G28" r:id="rId27" xr:uid="{15FB2B6A-5328-4F63-B57D-726C648AA529}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId27"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Single number, single numer III and longest palindromic substring
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive\Projects\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B6647F-556B-4C33-8A66-7495C64BEFDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D369E37-7546-467A-82E4-1B2A87CB108C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11145" yWindow="3885" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -274,6 +274,24 @@
   </si>
   <si>
     <t>441 - Arranging Coins</t>
+  </si>
+  <si>
+    <t>Single Number</t>
+  </si>
+  <si>
+    <t>136 - Single Number</t>
+  </si>
+  <si>
+    <t>Single Number III</t>
+  </si>
+  <si>
+    <t>260 - Single Number III</t>
+  </si>
+  <si>
+    <t>Longest Palindromic Substring</t>
+  </si>
+  <si>
+    <t>5 - Longest Palindromic Substring</t>
   </si>
 </sst>
 </file>
@@ -639,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,9 +1411,78 @@
         <v>82</v>
       </c>
     </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" t="s">
+        <v>33</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F32">
+  <conditionalFormatting sqref="D2:G8 D9:F35">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1407,16 +1494,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F32" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F35" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C32" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C35" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B32" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B35" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D32" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D35" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1452,8 +1539,11 @@
     <hyperlink ref="G30" r:id="rId29" xr:uid="{8461173A-A52B-483D-8D62-0CE26C939FF2}"/>
     <hyperlink ref="G31" r:id="rId30" xr:uid="{A7B26997-0FD7-4C90-A3FE-CCAFF3506658}"/>
     <hyperlink ref="G32" r:id="rId31" xr:uid="{E0169EE5-4CAC-40A9-8EEF-4829DE608E42}"/>
+    <hyperlink ref="G33" r:id="rId32" xr:uid="{E22C579B-40FB-4AA5-A79A-1FDD5870E3A6}"/>
+    <hyperlink ref="G34" r:id="rId33" xr:uid="{161C243A-7676-460E-84CE-00F11A394579}"/>
+    <hyperlink ref="G35" r:id="rId34" xr:uid="{2A04CDA6-6610-417C-9FFE-A355A661060D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId32"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId35"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Unique Binary Search Trees
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive\Projects\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D369E37-7546-467A-82E4-1B2A87CB108C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9CE776-79E5-485B-9B6F-1BA9FFBF6DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11145" yWindow="3885" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="91">
   <si>
     <t>Name</t>
   </si>
@@ -292,6 +292,12 @@
   </si>
   <si>
     <t>5 - Longest Palindromic Substring</t>
+  </si>
+  <si>
+    <t>Unique Binary Search Trees</t>
+  </si>
+  <si>
+    <t>96 - Unique Binary Search Trees</t>
   </si>
 </sst>
 </file>
@@ -657,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1480,9 +1486,32 @@
         <v>88</v>
       </c>
     </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36" t="s">
+        <v>30</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F35">
+  <conditionalFormatting sqref="D2:G8 D9:F36">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1494,16 +1523,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F35" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F36" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C35" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C36" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B35" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B36" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D35" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D36" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1542,8 +1571,9 @@
     <hyperlink ref="G33" r:id="rId32" xr:uid="{E22C579B-40FB-4AA5-A79A-1FDD5870E3A6}"/>
     <hyperlink ref="G34" r:id="rId33" xr:uid="{161C243A-7676-460E-84CE-00F11A394579}"/>
     <hyperlink ref="G35" r:id="rId34" xr:uid="{2A04CDA6-6610-417C-9FFE-A355A661060D}"/>
+    <hyperlink ref="G36" r:id="rId35" xr:uid="{7BE9D952-BDCF-4C89-B977-CEB38A1B5060}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId35"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId36"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Letter Combinations of a Phone Number
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive\Projects\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9CE776-79E5-485B-9B6F-1BA9FFBF6DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1809C92-73C2-4C3F-817B-35C2F0937792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11145" yWindow="3885" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="93">
   <si>
     <t>Name</t>
   </si>
@@ -298,6 +298,12 @@
   </si>
   <si>
     <t>96 - Unique Binary Search Trees</t>
+  </si>
+  <si>
+    <t>Letter Combinations of a Phone Number</t>
+  </si>
+  <si>
+    <t>17 - Letter Combinations of a Phone Number</t>
   </si>
 </sst>
 </file>
@@ -663,9 +669,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
@@ -1509,9 +1515,32 @@
         <v>90</v>
       </c>
     </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" t="s">
+        <v>30</v>
+      </c>
+      <c r="F37" t="s">
+        <v>6</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F36">
+  <conditionalFormatting sqref="D2:G8 D9:F37">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1523,16 +1552,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F36" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F37" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C36" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C37" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B36" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B37" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D36" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D37" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1572,8 +1601,9 @@
     <hyperlink ref="G34" r:id="rId33" xr:uid="{161C243A-7676-460E-84CE-00F11A394579}"/>
     <hyperlink ref="G35" r:id="rId34" xr:uid="{2A04CDA6-6610-417C-9FFE-A355A661060D}"/>
     <hyperlink ref="G36" r:id="rId35" xr:uid="{7BE9D952-BDCF-4C89-B977-CEB38A1B5060}"/>
+    <hyperlink ref="G37" r:id="rId36" xr:uid="{023255E4-203C-4492-9DE7-8472BE628683}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId36"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId37"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Linked List Cycle
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive\Projects\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1809C92-73C2-4C3F-817B-35C2F0937792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9348E81-6AE3-46CF-A87A-0A7FC7E00125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11145" yWindow="3885" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="95">
   <si>
     <t>Name</t>
   </si>
@@ -304,6 +304,12 @@
   </si>
   <si>
     <t>17 - Letter Combinations of a Phone Number</t>
+  </si>
+  <si>
+    <t>Linked List Cycle</t>
+  </si>
+  <si>
+    <t>141 - Linked List Cycle</t>
   </si>
 </sst>
 </file>
@@ -669,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1538,9 +1544,32 @@
         <v>92</v>
       </c>
     </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" t="s">
+        <v>6</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F37">
+  <conditionalFormatting sqref="D2:G8 D9:F38">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1552,16 +1581,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F37" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F38" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C37" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C38" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B37" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B38" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D37" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D38" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1602,8 +1631,9 @@
     <hyperlink ref="G35" r:id="rId34" xr:uid="{2A04CDA6-6610-417C-9FFE-A355A661060D}"/>
     <hyperlink ref="G36" r:id="rId35" xr:uid="{7BE9D952-BDCF-4C89-B977-CEB38A1B5060}"/>
     <hyperlink ref="G37" r:id="rId36" xr:uid="{023255E4-203C-4492-9DE7-8472BE628683}"/>
+    <hyperlink ref="G38" r:id="rId37" xr:uid="{9C786972-A475-436D-B233-D82BD67EDD61}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId37"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId38"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Remove Linked List Elements
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive\Projects\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9348E81-6AE3-46CF-A87A-0A7FC7E00125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E309FE-3144-4E5E-8394-F6DF93DAD3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11145" yWindow="3885" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="97">
   <si>
     <t>Name</t>
   </si>
@@ -310,6 +310,12 @@
   </si>
   <si>
     <t>141 - Linked List Cycle</t>
+  </si>
+  <si>
+    <t>Remove Linked List Elements</t>
+  </si>
+  <si>
+    <t>203 - Remove Linked List Elements</t>
   </si>
 </sst>
 </file>
@@ -675,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1567,9 +1573,32 @@
         <v>94</v>
       </c>
     </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" t="s">
+        <v>6</v>
+      </c>
+      <c r="F39" t="s">
+        <v>30</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F38">
+  <conditionalFormatting sqref="D2:G8 D9:F39">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1581,16 +1610,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F38" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F39" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C38" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C39" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B38" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B39" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D38" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D39" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1632,8 +1661,9 @@
     <hyperlink ref="G36" r:id="rId35" xr:uid="{7BE9D952-BDCF-4C89-B977-CEB38A1B5060}"/>
     <hyperlink ref="G37" r:id="rId36" xr:uid="{023255E4-203C-4492-9DE7-8472BE628683}"/>
     <hyperlink ref="G38" r:id="rId37" xr:uid="{9C786972-A475-436D-B233-D82BD67EDD61}"/>
+    <hyperlink ref="G39" r:id="rId38" xr:uid="{89DBF872-BE4E-43DC-BE08-5E84D16FFAFF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId38"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId39"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Merge k sorted Lists
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive\Projects\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E309FE-3144-4E5E-8394-F6DF93DAD3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE5626D-5B02-4EE3-9F15-A167612743A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11145" yWindow="3885" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="101">
   <si>
     <t>Name</t>
   </si>
@@ -141,9 +141,6 @@
     <t>Min Stack</t>
   </si>
   <si>
-    <t>Heap</t>
-  </si>
-  <si>
     <t>155 - Min Stack</t>
   </si>
   <si>
@@ -316,6 +313,21 @@
   </si>
   <si>
     <t>203 - Remove Linked List Elements</t>
+  </si>
+  <si>
+    <t>Class Design</t>
+  </si>
+  <si>
+    <t>Daily Temperatures</t>
+  </si>
+  <si>
+    <t>739 - Daily Temperatures</t>
+  </si>
+  <si>
+    <t>Merge k Sorted Lists</t>
+  </si>
+  <si>
+    <t>23 - Merge k Sorted Lists</t>
   </si>
 </sst>
 </file>
@@ -681,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P41" sqref="P41"/>
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,27 +969,27 @@
         <v>37</v>
       </c>
       <c r="B12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -995,12 +1007,12 @@
         <v>6</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
@@ -1018,12 +1030,12 @@
         <v>30</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -1041,12 +1053,12 @@
         <v>30</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
@@ -1064,12 +1076,12 @@
         <v>6</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
@@ -1087,12 +1099,12 @@
         <v>33</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
@@ -1110,61 +1122,61 @@
         <v>30</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
         <v>52</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="B20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
         <v>57</v>
-      </c>
-      <c r="B21" t="s">
-        <v>58</v>
       </c>
       <c r="C21" t="s">
         <v>12</v>
@@ -1179,12 +1191,12 @@
         <v>33</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
@@ -1202,35 +1214,35 @@
         <v>30</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" t="s">
         <v>62</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" t="s">
-        <v>6</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
         <v>19</v>
@@ -1248,12 +1260,12 @@
         <v>6</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
         <v>11</v>
@@ -1271,12 +1283,12 @@
         <v>6</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B26" t="s">
         <v>32</v>
@@ -1294,12 +1306,12 @@
         <v>30</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s">
         <v>32</v>
@@ -1317,12 +1329,12 @@
         <v>6</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
         <v>32</v>
@@ -1340,12 +1352,12 @@
         <v>6</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B29" t="s">
         <v>32</v>
@@ -1363,12 +1375,12 @@
         <v>6</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
@@ -1386,61 +1398,61 @@
         <v>6</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="B31" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" t="s">
-        <v>6</v>
-      </c>
-      <c r="F31" t="s">
-        <v>6</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="B32" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" t="s">
-        <v>6</v>
-      </c>
-      <c r="F32" t="s">
-        <v>30</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" t="s">
         <v>12</v>
@@ -1455,15 +1467,15 @@
         <v>33</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C34" t="s">
         <v>12</v>
@@ -1478,12 +1490,12 @@
         <v>33</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B35" t="s">
         <v>11</v>
@@ -1501,12 +1513,12 @@
         <v>6</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B36" t="s">
         <v>32</v>
@@ -1524,12 +1536,12 @@
         <v>30</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B37" t="s">
         <v>11</v>
@@ -1547,12 +1559,12 @@
         <v>6</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B38" t="s">
         <v>19</v>
@@ -1570,12 +1582,12 @@
         <v>6</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B39" t="s">
         <v>19</v>
@@ -1593,12 +1605,58 @@
         <v>30</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>99</v>
+      </c>
+      <c r="B40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" t="s">
+        <v>33</v>
+      </c>
+      <c r="F40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" t="s">
+        <v>30</v>
+      </c>
+      <c r="F41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F39">
+  <conditionalFormatting sqref="D2:G8 D9:F41">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1610,17 +1668,17 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F39" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F41" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C39" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C41" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B39" xr:uid="{DFFF5E79-B694-4F96-A9A2-484A044F8590}">
-      <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D41" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+      <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D39" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
-      <formula1>"Yes, No"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B41" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
+      <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap, Class Design"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -1662,8 +1720,10 @@
     <hyperlink ref="G37" r:id="rId36" xr:uid="{023255E4-203C-4492-9DE7-8472BE628683}"/>
     <hyperlink ref="G38" r:id="rId37" xr:uid="{9C786972-A475-436D-B233-D82BD67EDD61}"/>
     <hyperlink ref="G39" r:id="rId38" xr:uid="{89DBF872-BE4E-43DC-BE08-5E84D16FFAFF}"/>
+    <hyperlink ref="G41" r:id="rId39" xr:uid="{7A0D172B-36D5-4910-B01D-1E997AB02BA8}"/>
+    <hyperlink ref="G40" r:id="rId40" xr:uid="{AC2835F4-3AFF-4957-9DD9-917C62D45EEB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId39"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId41"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Length of Last Word and Min Cost Climbing Stairs
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive\Projects\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE5626D-5B02-4EE3-9F15-A167612743A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7B0AB2-043D-47CC-AE4D-E2F03D8A4D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11145" yWindow="3885" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="105">
   <si>
     <t>Name</t>
   </si>
@@ -328,6 +328,18 @@
   </si>
   <si>
     <t>23 - Merge k Sorted Lists</t>
+  </si>
+  <si>
+    <t>Min Cost Climbing Stairs</t>
+  </si>
+  <si>
+    <t>746 - Min Cost Climbing Stairs</t>
+  </si>
+  <si>
+    <t>Length of Last Word</t>
+  </si>
+  <si>
+    <t>58 - Length of Last Word</t>
   </si>
 </sst>
 </file>
@@ -693,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1654,9 +1666,55 @@
         <v>98</v>
       </c>
     </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42" t="s">
+        <v>30</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>103</v>
+      </c>
+      <c r="B43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" t="s">
+        <v>6</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F41">
+  <conditionalFormatting sqref="D2:G8 D9:F43">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1668,16 +1726,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F41" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F43" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C41" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C43" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D41" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D43" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B41" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B43" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap, Class Design"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1722,8 +1780,10 @@
     <hyperlink ref="G39" r:id="rId38" xr:uid="{89DBF872-BE4E-43DC-BE08-5E84D16FFAFF}"/>
     <hyperlink ref="G41" r:id="rId39" xr:uid="{7A0D172B-36D5-4910-B01D-1E997AB02BA8}"/>
     <hyperlink ref="G40" r:id="rId40" xr:uid="{AC2835F4-3AFF-4957-9DD9-917C62D45EEB}"/>
+    <hyperlink ref="G42" r:id="rId41" xr:uid="{0EB88B39-4963-4901-B53D-71DD4FAD84EF}"/>
+    <hyperlink ref="G43" r:id="rId42" xr:uid="{C21F1911-AD71-49FC-9170-13B242ECC7CE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId41"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId43"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Insert Delete GetRandom O(1)
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive\Projects\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7B0AB2-043D-47CC-AE4D-E2F03D8A4D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF20433-085E-43E2-A4FD-BB106797CFB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11145" yWindow="3885" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="107">
   <si>
     <t>Name</t>
   </si>
@@ -340,6 +340,12 @@
   </si>
   <si>
     <t>58 - Length of Last Word</t>
+  </si>
+  <si>
+    <t>Insert Delete GetRandom O(1)</t>
+  </si>
+  <si>
+    <t>380 - Insert Delete GetRandom O(1)</t>
   </si>
 </sst>
 </file>
@@ -705,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="M44" sqref="M44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1712,9 +1718,35 @@
         <v>104</v>
       </c>
     </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" t="s">
+        <v>30</v>
+      </c>
+      <c r="F44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G45" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F43">
+  <conditionalFormatting sqref="D2:G8 D9:F44">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1726,16 +1758,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F43" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F44" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C43" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C44" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D43" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D44" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B43" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B44" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap, Class Design"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1782,8 +1814,9 @@
     <hyperlink ref="G40" r:id="rId40" xr:uid="{AC2835F4-3AFF-4957-9DD9-917C62D45EEB}"/>
     <hyperlink ref="G42" r:id="rId41" xr:uid="{0EB88B39-4963-4901-B53D-71DD4FAD84EF}"/>
     <hyperlink ref="G43" r:id="rId42" xr:uid="{C21F1911-AD71-49FC-9170-13B242ECC7CE}"/>
+    <hyperlink ref="G44" r:id="rId43" xr:uid="{0BD462C8-7E3C-465E-A8E9-297FE9125FAB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId43"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId44"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add First Bad Version
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Projects\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA05D96C-9BAC-44C2-A16D-3279C4DE3B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585641D5-CA14-4742-80BF-6B2A66100ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="4050" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8775" yWindow="5670" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="115">
   <si>
     <t>Name</t>
   </si>
@@ -364,6 +364,12 @@
   </si>
   <si>
     <t>704 - Binary Search</t>
+  </si>
+  <si>
+    <t>First Bad Version</t>
+  </si>
+  <si>
+    <t>278 - First Bad Version</t>
   </si>
 </sst>
 </file>
@@ -729,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="N46" sqref="N46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1828,9 +1834,32 @@
         <v>112</v>
       </c>
     </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48" t="s">
+        <v>6</v>
+      </c>
+      <c r="F48" t="s">
+        <v>6</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F47">
+  <conditionalFormatting sqref="D2:G8 D9:F48">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1842,16 +1871,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F47" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F48" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C47" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C48" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D47" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D48" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B47" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B48" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap, Class Design"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1902,8 +1931,9 @@
     <hyperlink ref="G45" r:id="rId44" xr:uid="{40B8E83E-AAF6-4219-B01B-DE178B001721}"/>
     <hyperlink ref="G46" r:id="rId45" xr:uid="{35BFF752-4915-48C0-9A3B-75F298196DC6}"/>
     <hyperlink ref="G47" r:id="rId46" xr:uid="{B447A5FC-546D-49EA-9BBA-BC399A2B545F}"/>
+    <hyperlink ref="G48" r:id="rId47" xr:uid="{D2CA49AD-2140-4021-9C33-6F42ACFA1343}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId47"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId48"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Search Insert Position
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Projects\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585641D5-CA14-4742-80BF-6B2A66100ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5316D83-F3BE-4BCE-8C0B-EA8EC828608D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8775" yWindow="5670" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8775" yWindow="5565" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="117">
   <si>
     <t>Name</t>
   </si>
@@ -370,6 +370,12 @@
   </si>
   <si>
     <t>278 - First Bad Version</t>
+  </si>
+  <si>
+    <t>Insert Search Position</t>
+  </si>
+  <si>
+    <t>35 - Search Insert Position</t>
   </si>
 </sst>
 </file>
@@ -735,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="N46" sqref="N46"/>
+      <selection activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1857,9 +1863,32 @@
         <v>114</v>
       </c>
     </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>115</v>
+      </c>
+      <c r="B49" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49" t="s">
+        <v>6</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F48">
+  <conditionalFormatting sqref="D2:G8 D9:F49">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1871,16 +1900,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F48" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F49" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C48" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C49" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D48" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D49" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B48" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B49" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap, Class Design"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1932,8 +1961,9 @@
     <hyperlink ref="G46" r:id="rId45" xr:uid="{35BFF752-4915-48C0-9A3B-75F298196DC6}"/>
     <hyperlink ref="G47" r:id="rId46" xr:uid="{B447A5FC-546D-49EA-9BBA-BC399A2B545F}"/>
     <hyperlink ref="G48" r:id="rId47" xr:uid="{D2CA49AD-2140-4021-9C33-6F42ACFA1343}"/>
+    <hyperlink ref="G49" r:id="rId48" xr:uid="{6D7D05A1-4303-4CA1-AAA2-19A749128C99}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId48"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId49"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Convert Binary Number in a Linked List to Integer
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Projects\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5316D83-F3BE-4BCE-8C0B-EA8EC828608D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AE672E-5C6F-4ED5-A068-B662606F8BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8775" yWindow="5565" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="119">
   <si>
     <t>Name</t>
   </si>
@@ -376,6 +376,12 @@
   </si>
   <si>
     <t>35 - Search Insert Position</t>
+  </si>
+  <si>
+    <t>Convert Binary Number in a Linked List to Integer</t>
+  </si>
+  <si>
+    <t>1290 - Convert Binary Number in a Linked List to Integer</t>
   </si>
 </sst>
 </file>
@@ -741,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="P43" sqref="P43"/>
+      <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1886,9 +1892,32 @@
         <v>116</v>
       </c>
     </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>117</v>
+      </c>
+      <c r="B50" t="s">
+        <v>52</v>
+      </c>
+      <c r="C50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50" t="s">
+        <v>6</v>
+      </c>
+      <c r="F50" t="s">
+        <v>6</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F49">
+  <conditionalFormatting sqref="D2:G8 D9:F50">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1900,16 +1929,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F49" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F50" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C49" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C50" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D49" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D50" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B49" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B50" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap, Class Design"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1962,8 +1991,9 @@
     <hyperlink ref="G47" r:id="rId46" xr:uid="{B447A5FC-546D-49EA-9BBA-BC399A2B545F}"/>
     <hyperlink ref="G48" r:id="rId47" xr:uid="{D2CA49AD-2140-4021-9C33-6F42ACFA1343}"/>
     <hyperlink ref="G49" r:id="rId48" xr:uid="{6D7D05A1-4303-4CA1-AAA2-19A749128C99}"/>
+    <hyperlink ref="G50" r:id="rId49" xr:uid="{738E0BB0-9D12-4940-B873-6030A34BF9D8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId49"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId50"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix build issues and add Squares of a Sorted Array
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Projects\ProgrammingPractice\LeetCode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F526A7-9143-4519-B9F6-FE657732528E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79572840-9522-458C-900C-9596426AA9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7350" yWindow="1425" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="125">
   <si>
     <t>Name</t>
   </si>
@@ -394,6 +394,12 @@
   </si>
   <si>
     <t>494 - Target Sum</t>
+  </si>
+  <si>
+    <t>Squares of a Sorted Array</t>
+  </si>
+  <si>
+    <t>977 - Squares of a Sorted Array</t>
   </si>
 </sst>
 </file>
@@ -759,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="T33" sqref="T33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1973,9 +1979,32 @@
         <v>122</v>
       </c>
     </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>123</v>
+      </c>
+      <c r="B53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" t="s">
+        <v>5</v>
+      </c>
+      <c r="E53" t="s">
+        <v>6</v>
+      </c>
+      <c r="F53" t="s">
+        <v>30</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F52">
+  <conditionalFormatting sqref="D2:G8 D9:F53">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -1987,16 +2016,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F52" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F53" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C52" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C53" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D52" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D53" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B52" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B53" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap, Class Design"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2052,8 +2081,9 @@
     <hyperlink ref="G50" r:id="rId49" xr:uid="{738E0BB0-9D12-4940-B873-6030A34BF9D8}"/>
     <hyperlink ref="G51" r:id="rId50" xr:uid="{E0C8B272-6CC4-4EF8-9345-20A70E0DC656}"/>
     <hyperlink ref="G52" r:id="rId51" xr:uid="{6F23535B-77FD-4F95-AC81-217039984CA1}"/>
+    <hyperlink ref="G53" r:id="rId52" xr:uid="{65E178F1-A80F-48FE-AFE8-06EF54380083}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId52"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId53"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Rotate Array and Move Zeroes
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\LeetCode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79572840-9522-458C-900C-9596426AA9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9EA0FC8-315E-4B5E-9325-CBD9805709C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7350" yWindow="1425" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="127">
   <si>
     <t>Name</t>
   </si>
@@ -400,6 +400,12 @@
   </si>
   <si>
     <t>977 - Squares of a Sorted Array</t>
+  </si>
+  <si>
+    <t>Rotate Array</t>
+  </si>
+  <si>
+    <t>189 - Rotate Array</t>
   </si>
 </sst>
 </file>
@@ -765,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J45" sqref="J45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2002,9 +2008,32 @@
         <v>124</v>
       </c>
     </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>125</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" t="s">
+        <v>30</v>
+      </c>
+      <c r="F54" t="s">
+        <v>30</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F53">
+  <conditionalFormatting sqref="D2:G8 D9:F54">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2016,16 +2045,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F53" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F54" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C53" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C54" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D53" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D54" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B53" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B54" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap, Class Design"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2082,8 +2111,9 @@
     <hyperlink ref="G51" r:id="rId50" xr:uid="{E0C8B272-6CC4-4EF8-9345-20A70E0DC656}"/>
     <hyperlink ref="G52" r:id="rId51" xr:uid="{6F23535B-77FD-4F95-AC81-217039984CA1}"/>
     <hyperlink ref="G53" r:id="rId52" xr:uid="{65E178F1-A80F-48FE-AFE8-06EF54380083}"/>
+    <hyperlink ref="G54" r:id="rId53" xr:uid="{FB592940-7477-42C3-91F0-E5E752940D0B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId53"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId54"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Two Sum II - Input Array Is Sorted
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9EA0FC8-315E-4B5E-9325-CBD9805709C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12D593D-BFD7-4F77-84E3-9142E8BED231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7350" yWindow="1425" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="131">
   <si>
     <t>Name</t>
   </si>
@@ -406,6 +406,18 @@
   </si>
   <si>
     <t>189 - Rotate Array</t>
+  </si>
+  <si>
+    <t>Move Zeroes</t>
+  </si>
+  <si>
+    <t>283 - Move Zeroes</t>
+  </si>
+  <si>
+    <t>Two Sum II - Input Array Is Sorted</t>
+  </si>
+  <si>
+    <t>167 - Two Sum II - Input Array Is Sorted</t>
   </si>
 </sst>
 </file>
@@ -771,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="K58" sqref="K58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2031,9 +2043,55 @@
         <v>126</v>
       </c>
     </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>127</v>
+      </c>
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" t="s">
+        <v>5</v>
+      </c>
+      <c r="E55" t="s">
+        <v>6</v>
+      </c>
+      <c r="F55" t="s">
+        <v>6</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>129</v>
+      </c>
+      <c r="B56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" t="s">
+        <v>12</v>
+      </c>
+      <c r="E56" t="s">
+        <v>6</v>
+      </c>
+      <c r="F56" t="s">
+        <v>6</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F54">
+  <conditionalFormatting sqref="D2:G8 D9:F56">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2045,16 +2103,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F54" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F56" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C54" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C56" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D54" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D56" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B54" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B56" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap, Class Design"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2112,8 +2170,10 @@
     <hyperlink ref="G52" r:id="rId51" xr:uid="{6F23535B-77FD-4F95-AC81-217039984CA1}"/>
     <hyperlink ref="G53" r:id="rId52" xr:uid="{65E178F1-A80F-48FE-AFE8-06EF54380083}"/>
     <hyperlink ref="G54" r:id="rId53" xr:uid="{FB592940-7477-42C3-91F0-E5E752940D0B}"/>
+    <hyperlink ref="G55" r:id="rId54" xr:uid="{A7374A14-D783-4EC2-BBAA-DA51D81DFC38}"/>
+    <hyperlink ref="G56" r:id="rId55" xr:uid="{DF4D60E0-26FA-49CD-BBBC-A0694869AF31}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId54"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId56"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Intersection of Two Arrays II
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12D593D-BFD7-4F77-84E3-9142E8BED231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F5BD6C-9496-4196-B616-C087694990D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7350" yWindow="1425" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10020" yWindow="1425" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="133">
   <si>
     <t>Name</t>
   </si>
@@ -418,6 +418,12 @@
   </si>
   <si>
     <t>167 - Two Sum II - Input Array Is Sorted</t>
+  </si>
+  <si>
+    <t> Intersection of Two Arrays II</t>
+  </si>
+  <si>
+    <t>350 - Intersection of Two Arrays II</t>
   </si>
 </sst>
 </file>
@@ -783,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="K58" sqref="K58"/>
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2089,9 +2095,32 @@
         <v>130</v>
       </c>
     </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>131</v>
+      </c>
+      <c r="B57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" t="s">
+        <v>12</v>
+      </c>
+      <c r="E57" t="s">
+        <v>6</v>
+      </c>
+      <c r="F57" t="s">
+        <v>6</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F56">
+  <conditionalFormatting sqref="D2:G8 D9:F57">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2103,16 +2132,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F56" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F57" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C56" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C57" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D56" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D57" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B56" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B57" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap, Class Design"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2172,8 +2201,9 @@
     <hyperlink ref="G54" r:id="rId53" xr:uid="{FB592940-7477-42C3-91F0-E5E752940D0B}"/>
     <hyperlink ref="G55" r:id="rId54" xr:uid="{A7374A14-D783-4EC2-BBAA-DA51D81DFC38}"/>
     <hyperlink ref="G56" r:id="rId55" xr:uid="{DF4D60E0-26FA-49CD-BBBC-A0694869AF31}"/>
+    <hyperlink ref="G57" r:id="rId56" xr:uid="{A9939275-6654-4961-9638-524932C2CCA7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId56"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId57"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Swap Nodes in Pairs
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F5BD6C-9496-4196-B616-C087694990D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC8CCE6-B247-448B-B77A-90A28DAF3D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10020" yWindow="1425" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="135">
   <si>
     <t>Name</t>
   </si>
@@ -424,6 +424,12 @@
   </si>
   <si>
     <t>350 - Intersection of Two Arrays II</t>
+  </si>
+  <si>
+    <t>Swap Nodes in Pairs</t>
+  </si>
+  <si>
+    <t>24 - Swap Nodes in Pairs</t>
   </si>
 </sst>
 </file>
@@ -789,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+      <selection activeCell="M62" sqref="M62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2118,9 +2124,32 @@
         <v>132</v>
       </c>
     </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>133</v>
+      </c>
+      <c r="B58" t="s">
+        <v>19</v>
+      </c>
+      <c r="C58" t="s">
+        <v>12</v>
+      </c>
+      <c r="D58" t="s">
+        <v>5</v>
+      </c>
+      <c r="E58" t="s">
+        <v>30</v>
+      </c>
+      <c r="F58" t="s">
+        <v>30</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F57">
+  <conditionalFormatting sqref="D2:G8 D9:F58">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2132,16 +2161,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F57" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F58" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C57" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C58" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D57" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D58" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B57" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B58" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap, Class Design"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2202,8 +2231,9 @@
     <hyperlink ref="G55" r:id="rId54" xr:uid="{A7374A14-D783-4EC2-BBAA-DA51D81DFC38}"/>
     <hyperlink ref="G56" r:id="rId55" xr:uid="{DF4D60E0-26FA-49CD-BBBC-A0694869AF31}"/>
     <hyperlink ref="G57" r:id="rId56" xr:uid="{A9939275-6654-4961-9638-524932C2CCA7}"/>
+    <hyperlink ref="G58" r:id="rId57" xr:uid="{E7F842BC-BE20-4B91-A89F-A3D539BAE5CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId57"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId58"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Minimum Absolute Difference
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D708BB09-3CB7-4085-A913-4DC86C8F10AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7084B866-C77C-4D17-BB09-D7F6B3F5AF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10020" yWindow="1425" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="139">
   <si>
     <t>Name</t>
   </si>
@@ -436,6 +436,12 @@
   </si>
   <si>
     <t>1446 - Consecutive Characters</t>
+  </si>
+  <si>
+    <t>Minimum Absolute Difference</t>
+  </si>
+  <si>
+    <t>1200 - Minimum Absolute Difference</t>
   </si>
 </sst>
 </file>
@@ -801,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="O61" sqref="O61"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="K55" sqref="K55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2176,9 +2182,32 @@
         <v>136</v>
       </c>
     </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>137</v>
+      </c>
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60" t="s">
+        <v>12</v>
+      </c>
+      <c r="E60" t="s">
+        <v>6</v>
+      </c>
+      <c r="F60" t="s">
+        <v>6</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F59">
+  <conditionalFormatting sqref="D2:G8 D9:F60">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2190,16 +2219,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F59" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F60" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C59" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C60" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D59" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D60" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B59" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B60" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap, Class Design"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2262,8 +2291,9 @@
     <hyperlink ref="G57" r:id="rId56" xr:uid="{A9939275-6654-4961-9638-524932C2CCA7}"/>
     <hyperlink ref="G58" r:id="rId57" xr:uid="{E7F842BC-BE20-4B91-A89F-A3D539BAE5CD}"/>
     <hyperlink ref="G59" r:id="rId58" xr:uid="{40463158-DAA5-4895-8D49-10CB753F3787}"/>
+    <hyperlink ref="G60" r:id="rId59" xr:uid="{529716AD-258B-46A3-839E-E8F87A26AE2B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId59"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId60"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add K Closest Points to Origin
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7084B866-C77C-4D17-BB09-D7F6B3F5AF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D061B5-BC72-4D31-A996-9B8F1C0E3359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10020" yWindow="1425" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="141">
   <si>
     <t>Name</t>
   </si>
@@ -442,6 +442,12 @@
   </si>
   <si>
     <t>1200 - Minimum Absolute Difference</t>
+  </si>
+  <si>
+    <t>K Closest Points to Origin</t>
+  </si>
+  <si>
+    <t>973 - K Closest Points to Origin</t>
   </si>
 </sst>
 </file>
@@ -807,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="K55" sqref="K55"/>
+      <selection activeCell="N46" sqref="N46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2205,9 +2211,32 @@
         <v>138</v>
       </c>
     </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>139</v>
+      </c>
+      <c r="B61" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" t="s">
+        <v>30</v>
+      </c>
+      <c r="F61" t="s">
+        <v>6</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F60">
+  <conditionalFormatting sqref="D2:G8 D9:F61">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2219,16 +2248,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F60" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F61" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C60" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C61" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D60" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D61" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B60" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B61" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap, Class Design"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2292,8 +2321,9 @@
     <hyperlink ref="G58" r:id="rId57" xr:uid="{E7F842BC-BE20-4B91-A89F-A3D539BAE5CD}"/>
     <hyperlink ref="G59" r:id="rId58" xr:uid="{40463158-DAA5-4895-8D49-10CB753F3787}"/>
     <hyperlink ref="G60" r:id="rId59" xr:uid="{529716AD-258B-46A3-839E-E8F87A26AE2B}"/>
+    <hyperlink ref="G61" r:id="rId60" xr:uid="{A7FEF6A2-B012-45A3-A14C-D3BD4BB6CA36}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId60"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId61"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Complement of Base 10 Integer and Number Complement
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D061B5-BC72-4D31-A996-9B8F1C0E3359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E526839-C298-4079-8AC4-5FADCA8CA3AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10020" yWindow="1425" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="145">
   <si>
     <t>Name</t>
   </si>
@@ -448,6 +448,18 @@
   </si>
   <si>
     <t>973 - K Closest Points to Origin</t>
+  </si>
+  <si>
+    <t>Complement of Base 10 Integer</t>
+  </si>
+  <si>
+    <t>Number Complement</t>
+  </si>
+  <si>
+    <t>1009 - Complement of Base 10 Integer</t>
+  </si>
+  <si>
+    <t>476 - Number Complement</t>
   </si>
 </sst>
 </file>
@@ -813,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="N46" sqref="N46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2234,9 +2246,55 @@
         <v>140</v>
       </c>
     </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>141</v>
+      </c>
+      <c r="B62" t="s">
+        <v>52</v>
+      </c>
+      <c r="C62" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62" t="s">
+        <v>12</v>
+      </c>
+      <c r="E62" t="s">
+        <v>6</v>
+      </c>
+      <c r="F62" t="s">
+        <v>6</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>142</v>
+      </c>
+      <c r="B63" t="s">
+        <v>52</v>
+      </c>
+      <c r="C63" t="s">
+        <v>12</v>
+      </c>
+      <c r="D63" t="s">
+        <v>12</v>
+      </c>
+      <c r="E63" t="s">
+        <v>6</v>
+      </c>
+      <c r="F63" t="s">
+        <v>6</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F61">
+  <conditionalFormatting sqref="D2:G8 D9:F63">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2248,16 +2306,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F61" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F63" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C61" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C63" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D61" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D63" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B61" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B63" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap, Class Design"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2322,8 +2380,10 @@
     <hyperlink ref="G59" r:id="rId58" xr:uid="{40463158-DAA5-4895-8D49-10CB753F3787}"/>
     <hyperlink ref="G60" r:id="rId59" xr:uid="{529716AD-258B-46A3-839E-E8F87A26AE2B}"/>
     <hyperlink ref="G61" r:id="rId60" xr:uid="{A7FEF6A2-B012-45A3-A14C-D3BD4BB6CA36}"/>
+    <hyperlink ref="G62" r:id="rId61" xr:uid="{52D5079F-4E70-4566-A831-D2C47D759501}"/>
+    <hyperlink ref="G63" r:id="rId62" xr:uid="{5ED7C51F-776C-40A8-934A-AF95A99382A4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId61"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId63"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Middle of the Linked List
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CF2D3E-F8E4-4C85-89E1-7457E69290DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952A2B73-9339-40DA-ACD0-6CECDFA499FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10020" yWindow="1425" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="149">
   <si>
     <t>Name</t>
   </si>
@@ -466,6 +466,12 @@
   </si>
   <si>
     <t>6 - Zigzag Conversion</t>
+  </si>
+  <si>
+    <t>Middle of the Linked List</t>
+  </si>
+  <si>
+    <t>876 - Middle of the Linked List</t>
   </si>
 </sst>
 </file>
@@ -831,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J47" sqref="J47"/>
+      <selection activeCell="P45" sqref="P45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2321,9 +2327,32 @@
         <v>146</v>
       </c>
     </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>147</v>
+      </c>
+      <c r="B65" t="s">
+        <v>19</v>
+      </c>
+      <c r="C65" t="s">
+        <v>12</v>
+      </c>
+      <c r="D65" t="s">
+        <v>12</v>
+      </c>
+      <c r="E65" t="s">
+        <v>6</v>
+      </c>
+      <c r="F65" t="s">
+        <v>6</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F64">
+  <conditionalFormatting sqref="D2:G8 D9:F65">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2335,16 +2364,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F64" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F65" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C64" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C65" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D64" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D65" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B64" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B65" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap, Class Design"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2412,8 +2441,9 @@
     <hyperlink ref="G62" r:id="rId61" xr:uid="{52D5079F-4E70-4566-A831-D2C47D759501}"/>
     <hyperlink ref="G63" r:id="rId62" xr:uid="{5ED7C51F-776C-40A8-934A-AF95A99382A4}"/>
     <hyperlink ref="G64" r:id="rId63" xr:uid="{C257C7F6-F5A4-4480-9EFC-1A9BD1B5FFA1}"/>
+    <hyperlink ref="G65" r:id="rId64" xr:uid="{36416745-B662-4F45-A71E-05838395244C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId64"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId65"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Valid Sudoku and clean up utility functions
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952A2B73-9339-40DA-ACD0-6CECDFA499FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B873F582-2884-4D2B-9117-E0049CA26EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10020" yWindow="1425" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="151">
   <si>
     <t>Name</t>
   </si>
@@ -472,6 +472,12 @@
   </si>
   <si>
     <t>876 - Middle of the Linked List</t>
+  </si>
+  <si>
+    <t>Valid Sudoku</t>
+  </si>
+  <si>
+    <t>36 - Valid Sudoku</t>
   </si>
 </sst>
 </file>
@@ -837,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="P45" sqref="P45"/>
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2350,9 +2356,32 @@
         <v>148</v>
       </c>
     </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>149</v>
+      </c>
+      <c r="B66" t="s">
+        <v>19</v>
+      </c>
+      <c r="C66" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" t="s">
+        <v>12</v>
+      </c>
+      <c r="E66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F66" t="s">
+        <v>6</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F65">
+  <conditionalFormatting sqref="D2:G8 D9:F66">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2364,16 +2393,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F65" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F66" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C65" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C66" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D65" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D66" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B65" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B66" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap, Class Design"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2442,8 +2471,9 @@
     <hyperlink ref="G63" r:id="rId62" xr:uid="{5ED7C51F-776C-40A8-934A-AF95A99382A4}"/>
     <hyperlink ref="G64" r:id="rId63" xr:uid="{C257C7F6-F5A4-4480-9EFC-1A9BD1B5FFA1}"/>
     <hyperlink ref="G65" r:id="rId64" xr:uid="{36416745-B662-4F45-A71E-05838395244C}"/>
+    <hyperlink ref="G66" r:id="rId65" xr:uid="{150B3A98-6BA7-4162-8A52-CD899AA9EE3F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId65"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId66"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More cleanup and add Populating Next Right Pointers in each Node II
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952A2B73-9339-40DA-ACD0-6CECDFA499FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0389F121-BC9D-4391-A6F2-25169C083FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10020" yWindow="1425" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="155">
   <si>
     <t>Name</t>
   </si>
@@ -472,6 +472,24 @@
   </si>
   <si>
     <t>876 - Middle of the Linked List</t>
+  </si>
+  <si>
+    <t>Valid Sudoku</t>
+  </si>
+  <si>
+    <t>36 - Valid Sudoku</t>
+  </si>
+  <si>
+    <t>Populating Next Right Pointers in Each Node</t>
+  </si>
+  <si>
+    <t>116 - Populating Next Right Pointers in Each Node</t>
+  </si>
+  <si>
+    <t>Populating Next Right Pointers in Each Node II</t>
+  </si>
+  <si>
+    <t>117 - Populating Next Right Pointers in Each Node II</t>
   </si>
 </sst>
 </file>
@@ -837,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="P45" sqref="P45"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="M63" sqref="M63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2350,9 +2368,78 @@
         <v>148</v>
       </c>
     </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>149</v>
+      </c>
+      <c r="B66" t="s">
+        <v>19</v>
+      </c>
+      <c r="C66" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" t="s">
+        <v>12</v>
+      </c>
+      <c r="E66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F66" t="s">
+        <v>6</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>151</v>
+      </c>
+      <c r="B67" t="s">
+        <v>32</v>
+      </c>
+      <c r="C67" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" t="s">
+        <v>5</v>
+      </c>
+      <c r="E67" t="s">
+        <v>30</v>
+      </c>
+      <c r="F67" t="s">
+        <v>30</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>153</v>
+      </c>
+      <c r="B68" t="s">
+        <v>32</v>
+      </c>
+      <c r="C68" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" t="s">
+        <v>12</v>
+      </c>
+      <c r="E68" t="s">
+        <v>30</v>
+      </c>
+      <c r="F68" t="s">
+        <v>30</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F65">
+  <conditionalFormatting sqref="D2:G8 D9:F68">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2364,16 +2451,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F65" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F68" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C65" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C68" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D65" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D68" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B65" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B68" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap, Class Design"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2442,8 +2529,11 @@
     <hyperlink ref="G63" r:id="rId62" xr:uid="{5ED7C51F-776C-40A8-934A-AF95A99382A4}"/>
     <hyperlink ref="G64" r:id="rId63" xr:uid="{C257C7F6-F5A4-4480-9EFC-1A9BD1B5FFA1}"/>
     <hyperlink ref="G65" r:id="rId64" xr:uid="{36416745-B662-4F45-A71E-05838395244C}"/>
+    <hyperlink ref="G66" r:id="rId65" xr:uid="{150B3A98-6BA7-4162-8A52-CD899AA9EE3F}"/>
+    <hyperlink ref="G67" r:id="rId66" xr:uid="{BC82AB54-4CD2-4EFA-8F79-21E3A82F28D6}"/>
+    <hyperlink ref="G68" r:id="rId67" xr:uid="{8A49092D-5825-42E0-BD22-D7052F8A2F78}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId65"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId68"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Robot Bounded In Circle
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB43839-A64B-4C43-804B-B6385B83F702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3E4248-5FD4-4FC4-9A64-A6CDFD5D5B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10020" yWindow="1425" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="156">
   <si>
     <t>Name</t>
   </si>
@@ -487,6 +487,12 @@
   </si>
   <si>
     <t>62 - Unique Paths</t>
+  </si>
+  <si>
+    <t>Robot Bounded In Circle</t>
+  </si>
+  <si>
+    <t>1041 - Robot Bounded In Circle</t>
   </si>
 </sst>
 </file>
@@ -852,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2434,9 +2440,32 @@
         <v>151</v>
       </c>
     </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>154</v>
+      </c>
+      <c r="B69" t="s">
+        <v>11</v>
+      </c>
+      <c r="C69" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" t="s">
+        <v>12</v>
+      </c>
+      <c r="E69" t="s">
+        <v>30</v>
+      </c>
+      <c r="F69" t="s">
+        <v>6</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F68">
+  <conditionalFormatting sqref="D2:G8 D9:F69">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2448,16 +2477,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F68" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F69" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C68" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C69" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D68" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D69" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B68" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B69" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap, Class Design"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2529,8 +2558,9 @@
     <hyperlink ref="G67" r:id="rId65" xr:uid="{BC82AB54-4CD2-4EFA-8F79-21E3A82F28D6}"/>
     <hyperlink ref="G68" r:id="rId66" xr:uid="{8A49092D-5825-42E0-BD22-D7052F8A2F78}"/>
     <hyperlink ref="G21" r:id="rId67" xr:uid="{F60BEC28-50D9-4AB9-8148-4E52EEF29C58}"/>
+    <hyperlink ref="G69" r:id="rId68" xr:uid="{6ACB39DD-5530-48EE-BDCF-893027D86A38}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId68"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId69"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Insert into a Binary Search Tree
</commit_message>
<xml_diff>
--- a/LeetCode/problems.xlsx
+++ b/LeetCode/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\ProgrammingPractice\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3E4248-5FD4-4FC4-9A64-A6CDFD5D5B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C724B99-C25D-43F5-9B6A-34BC0C6A116F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10020" yWindow="1425" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="158">
   <si>
     <t>Name</t>
   </si>
@@ -493,6 +493,12 @@
   </si>
   <si>
     <t>1041 - Robot Bounded In Circle</t>
+  </si>
+  <si>
+    <t>Insert into a Binary Search Tree</t>
+  </si>
+  <si>
+    <t>701 - Insert into a Binary Search Tree</t>
   </si>
 </sst>
 </file>
@@ -858,10 +864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="L49" sqref="L49"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L51" sqref="L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2463,9 +2469,32 @@
         <v>155</v>
       </c>
     </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>156</v>
+      </c>
+      <c r="B70" t="s">
+        <v>32</v>
+      </c>
+      <c r="C70" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70" t="s">
+        <v>12</v>
+      </c>
+      <c r="E70" t="s">
+        <v>30</v>
+      </c>
+      <c r="F70" t="s">
+        <v>6</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D2:G8 D9:F69">
+  <conditionalFormatting sqref="D2:G8 D9:F70">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hard"</formula>
     </cfRule>
@@ -2477,16 +2506,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F69" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F70" xr:uid="{8D0F090F-218A-4D2E-AC02-40E613B420C8}">
       <formula1>"Easy, Medium, Hard"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C69" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C70" xr:uid="{C4BAC5F9-E5B3-46BA-8B18-DA12EDDD23B0}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D69" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D70" xr:uid="{533ED654-6D73-4810-B587-12605A1BD8A9}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B69" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B70" xr:uid="{C760D8CE-914D-4FD8-B266-B80F2C10E7B3}">
       <formula1>"Array, Binary, Dynamic Programming, Graph, Interval, Linked List, Matrix, String, Tree, Heap, Class Design"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2559,8 +2588,9 @@
     <hyperlink ref="G68" r:id="rId66" xr:uid="{8A49092D-5825-42E0-BD22-D7052F8A2F78}"/>
     <hyperlink ref="G21" r:id="rId67" xr:uid="{F60BEC28-50D9-4AB9-8148-4E52EEF29C58}"/>
     <hyperlink ref="G69" r:id="rId68" xr:uid="{6ACB39DD-5530-48EE-BDCF-893027D86A38}"/>
+    <hyperlink ref="G70" r:id="rId69" xr:uid="{3AB22C19-BC60-4E89-8C9A-C4D6114C8FAD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId69"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId70"/>
 </worksheet>
 </file>
</xml_diff>